<commit_message>
Algoritmo para slice and dice funcionando
</commit_message>
<xml_diff>
--- a/ocupacao.xlsx
+++ b/ocupacao.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="1830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -709,7 +709,22 @@
         <v>266</v>
       </c>
       <c r="O2">
-        <v>79</v>
+        <v>225</v>
+      </c>
+      <c r="P2">
+        <v>274</v>
+      </c>
+      <c r="Q2">
+        <v>260</v>
+      </c>
+      <c r="R2">
+        <v>249</v>
+      </c>
+      <c r="S2">
+        <v>248</v>
+      </c>
+      <c r="T2">
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
@@ -753,7 +768,22 @@
         <v>266</v>
       </c>
       <c r="O3">
-        <v>79</v>
+        <v>225</v>
+      </c>
+      <c r="P3">
+        <v>260</v>
+      </c>
+      <c r="Q3">
+        <v>248</v>
+      </c>
+      <c r="R3">
+        <v>253</v>
+      </c>
+      <c r="S3">
+        <v>250</v>
+      </c>
+      <c r="T3">
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
@@ -797,7 +827,22 @@
         <v>264</v>
       </c>
       <c r="O4">
-        <v>89</v>
+        <v>234</v>
+      </c>
+      <c r="P4">
+        <v>255</v>
+      </c>
+      <c r="Q4">
+        <v>265</v>
+      </c>
+      <c r="R4">
+        <v>267</v>
+      </c>
+      <c r="S4">
+        <v>254</v>
+      </c>
+      <c r="T4">
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
@@ -841,7 +886,22 @@
         <v>275</v>
       </c>
       <c r="O5">
-        <v>88</v>
+        <v>244</v>
+      </c>
+      <c r="P5">
+        <v>258</v>
+      </c>
+      <c r="Q5">
+        <v>254</v>
+      </c>
+      <c r="R5">
+        <v>243</v>
+      </c>
+      <c r="S5">
+        <v>244</v>
+      </c>
+      <c r="T5">
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
@@ -885,7 +945,22 @@
         <v>266</v>
       </c>
       <c r="O6">
-        <v>90</v>
+        <v>242</v>
+      </c>
+      <c r="P6">
+        <v>265</v>
+      </c>
+      <c r="Q6">
+        <v>241</v>
+      </c>
+      <c r="R6">
+        <v>274</v>
+      </c>
+      <c r="S6">
+        <v>245</v>
+      </c>
+      <c r="T6">
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
@@ -929,7 +1004,22 @@
         <v>259</v>
       </c>
       <c r="O7">
-        <v>85</v>
+        <v>236</v>
+      </c>
+      <c r="P7">
+        <v>272</v>
+      </c>
+      <c r="Q7">
+        <v>256</v>
+      </c>
+      <c r="R7">
+        <v>261</v>
+      </c>
+      <c r="S7">
+        <v>258</v>
+      </c>
+      <c r="T7">
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
@@ -973,7 +1063,22 @@
         <v>261</v>
       </c>
       <c r="O8">
-        <v>73</v>
+        <v>229</v>
+      </c>
+      <c r="P8">
+        <v>255</v>
+      </c>
+      <c r="Q8">
+        <v>250</v>
+      </c>
+      <c r="R8">
+        <v>260</v>
+      </c>
+      <c r="S8">
+        <v>268</v>
+      </c>
+      <c r="T8">
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
@@ -1017,7 +1122,22 @@
         <v>262</v>
       </c>
       <c r="O9">
-        <v>86</v>
+        <v>229</v>
+      </c>
+      <c r="P9">
+        <v>267</v>
+      </c>
+      <c r="Q9">
+        <v>236</v>
+      </c>
+      <c r="R9">
+        <v>279</v>
+      </c>
+      <c r="S9">
+        <v>249</v>
+      </c>
+      <c r="T9">
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
@@ -1061,7 +1181,22 @@
         <v>271</v>
       </c>
       <c r="O10">
-        <v>81</v>
+        <v>226</v>
+      </c>
+      <c r="P10">
+        <v>258</v>
+      </c>
+      <c r="Q10">
+        <v>258</v>
+      </c>
+      <c r="R10">
+        <v>257</v>
+      </c>
+      <c r="S10">
+        <v>260</v>
+      </c>
+      <c r="T10">
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
@@ -1105,7 +1240,22 @@
         <v>265</v>
       </c>
       <c r="O11">
-        <v>79</v>
+        <v>229</v>
+      </c>
+      <c r="P11">
+        <v>255</v>
+      </c>
+      <c r="Q11">
+        <v>255</v>
+      </c>
+      <c r="R11">
+        <v>258</v>
+      </c>
+      <c r="S11">
+        <v>232</v>
+      </c>
+      <c r="T11">
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.25">
@@ -1149,7 +1299,22 @@
         <v>259</v>
       </c>
       <c r="O12">
-        <v>82</v>
+        <v>245</v>
+      </c>
+      <c r="P12">
+        <v>279</v>
+      </c>
+      <c r="Q12">
+        <v>251</v>
+      </c>
+      <c r="R12">
+        <v>261</v>
+      </c>
+      <c r="S12">
+        <v>233</v>
+      </c>
+      <c r="T12">
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.25">
@@ -1193,7 +1358,22 @@
         <v>275</v>
       </c>
       <c r="O13">
-        <v>84</v>
+        <v>231</v>
+      </c>
+      <c r="P13">
+        <v>263</v>
+      </c>
+      <c r="Q13">
+        <v>265</v>
+      </c>
+      <c r="R13">
+        <v>243</v>
+      </c>
+      <c r="S13">
+        <v>264</v>
+      </c>
+      <c r="T13">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>